<commit_message>
bar chart add and logo change
</commit_message>
<xml_diff>
--- a/src/assets/champion_counter.xlsx
+++ b/src/assets/champion_counter.xlsx
@@ -607,7 +607,7 @@
         <v>Brazil</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -735,7 +735,7 @@
         <v>Spain</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">

</xml_diff>

<commit_message>
data get from google sheets
</commit_message>
<xml_diff>
--- a/src/assets/champion_counter.xlsx
+++ b/src/assets/champion_counter.xlsx
@@ -607,7 +607,7 @@
         <v>Brazil</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27">
@@ -735,7 +735,7 @@
         <v>Spain</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">

</xml_diff>